<commit_message>
updated submodules + parts
</commit_message>
<xml_diff>
--- a/PCB/CollatedParts.xlsx
+++ b/PCB/CollatedParts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s/Desktop/nvf/NVF2-DataAcq-Hardware/PCB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC8BADD-9814-2248-BD55-8EC48D886AA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71296CF2-AD48-DA40-A939-2261DE97DF9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="760" windowWidth="29160" windowHeight="18880" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-8160" yWindow="-21100" windowWidth="38400" windowHeight="21100" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Connectors" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="243">
   <si>
     <t>Out Of Stock</t>
   </si>
@@ -730,6 +730,52 @@
   </si>
   <si>
     <t>https://datasheet.lcsc.com/lcsc/2206010130_UNI-ROYAL-Uniroyal-Elec-0603WAF100JT5E_C22859.pdf</t>
+  </si>
+  <si>
+    <t>3362P-1-103LF</t>
+  </si>
+  <si>
+    <t>3362P</t>
+  </si>
+  <si>
+    <t>C58159</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/2304140030_BOURNS-3362P-1-103LF_C58159.pdf</t>
+  </si>
+  <si>
+    <t>STM32F072CBT6</t>
+  </si>
+  <si>
+    <t>Microcontroller</t>
+  </si>
+  <si>
+    <t>128KB Cortex-M0 16KB 48MHz</t>
+  </si>
+  <si>
+    <t>LQFP-48(7x7)</t>
+  </si>
+  <si>
+    <t>C81720</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/2304140030_STMicroelectronics-STM32F072CBT6_C81720.pdf</t>
+  </si>
+  <si>
+    <t>STM32H723ZGT6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+1MB Cortex-M7 564KB 550MHz </t>
+  </si>
+  <si>
+    <t>LQFP-144(20x20)</t>
+  </si>
+  <si>
+    <t>C730146</t>
+  </si>
+  <si>
+    <t>https://datasheet.lcsc.com/lcsc/2009021033_STMicroelectronics-STM32H723ZGT6_C730146.pdf</t>
   </si>
 </sst>
 </file>
@@ -1764,17 +1810,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A3:AMJ40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.6640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="19.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" style="2" customWidth="1"/>
-    <col min="5" max="7" width="9.1640625" style="2"/>
+    <col min="3" max="3" width="25.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9.1640625" style="2"/>
     <col min="8" max="8" width="39.6640625" style="11" customWidth="1"/>
     <col min="9" max="1024" width="9.1640625" style="2"/>
   </cols>
@@ -1812,68 +1859,68 @@
     </row>
     <row r="4" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
-        <f t="shared" ref="A4:A40" si="0">ROW()-ROW($A$3)</f>
+        <f>ROW()-ROW($A$3)</f>
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>223</v>
+        <v>139</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>75</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW($A$3)</f>
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>138</v>
+        <v>119</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>140</v>
+        <v>79</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>75</v>
+        <v>121</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW($A$3)</f>
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>120</v>
@@ -1882,52 +1929,52 @@
         <v>79</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>81</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW($A$3)</f>
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>120</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>79</v>
+        <v>111</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>81</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW($A$3)</f>
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>120</v>
@@ -1936,25 +1983,25 @@
         <v>111</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>81</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW($A$3)</f>
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>120</v>
@@ -1963,52 +2010,52 @@
         <v>111</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>81</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW($A$3)</f>
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>120</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>111</v>
+        <v>79</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>81</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW($A$3)</f>
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>134</v>
+        <v>215</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>135</v>
+        <v>221</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>120</v>
@@ -2017,187 +2064,187 @@
         <v>79</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>136</v>
+        <v>216</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>81</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>186</v>
+        <v>222</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW($A$3)</f>
         <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>215</v>
+        <v>146</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>221</v>
+        <v>147</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>120</v>
+        <v>189</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>79</v>
+        <v>148</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>216</v>
+        <v>149</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>81</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>222</v>
+        <v>187</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW($A$3)</f>
         <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>146</v>
+        <v>113</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>147</v>
+        <v>114</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>189</v>
+        <v>115</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>148</v>
+        <v>116</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>149</v>
+        <v>117</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>81</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW($A$3)</f>
         <v>11</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>113</v>
+        <v>152</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>114</v>
+        <v>153</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>115</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>116</v>
+        <v>154</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>117</v>
+        <v>155</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>81</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW($A$3)</f>
         <v>12</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>152</v>
+        <v>108</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>153</v>
+        <v>109</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>154</v>
+        <v>111</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>155</v>
+        <v>112</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>81</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW($A$3)</f>
         <v>13</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>108</v>
+      <c r="B16" s="8" t="s">
+        <v>204</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>109</v>
+        <v>205</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>111</v>
+        <v>206</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>207</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>112</v>
+        <v>208</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>178</v>
+        <v>209</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW($A$3)</f>
         <v>14</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>204</v>
+      <c r="B17" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>205</v>
+        <v>101</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>207</v>
+        <v>102</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>103</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>208</v>
+        <v>104</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>209</v>
+        <v>177</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW($A$3)</f>
         <v>15</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>102</v>
@@ -2206,241 +2253,241 @@
         <v>103</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>81</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW($A$3)</f>
         <v>16</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>105</v>
+      <c r="B19" s="8" t="s">
+        <v>94</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>81</v>
+        <v>96</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>176</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW($A$3)</f>
         <v>17</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>94</v>
+        <v>191</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>95</v>
+        <v>150</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="E20" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>98</v>
+      <c r="E20" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>190</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>75</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>99</v>
+        <v>192</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW($A$3)</f>
         <v>18</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>150</v>
+        <v>201</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>151</v>
+        <v>201</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>202</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="G21" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="G21" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="H21" s="11" t="s">
-        <v>192</v>
+      <c r="H21" s="12" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW($A$3)</f>
         <v>19</v>
       </c>
-      <c r="B22" s="8" t="s">
-        <v>200</v>
+      <c r="B22" s="2" t="s">
+        <v>232</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>201</v>
+        <v>234</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>202</v>
+        <v>233</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>235</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>203</v>
+        <v>236</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="H22" s="12" t="s">
-        <v>199</v>
+      <c r="H22" s="11" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW($A$3)</f>
         <v>20</v>
       </c>
-      <c r="B23" s="8" t="s">
-        <v>210</v>
+      <c r="B23" s="2" t="s">
+        <v>238</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>211</v>
+        <v>239</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>212</v>
+        <v>233</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>224</v>
+        <v>240</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>213</v>
+        <v>241</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>75</v>
       </c>
       <c r="H23" s="11" t="s">
-        <v>214</v>
+        <v>242</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW($A$3)</f>
         <v>21</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>76</v>
+        <v>142</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>77</v>
+        <v>143</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>78</v>
+        <v>223</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>79</v>
+        <v>144</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>81</v>
+        <v>145</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW($A$3)</f>
         <v>22</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>83</v>
+      <c r="B25" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>211</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>78</v>
+        <v>212</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>79</v>
+        <v>224</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>84</v>
+        <v>213</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>171</v>
+        <v>214</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW($A$3)</f>
         <v>23</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>86</v>
+        <v>228</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>211</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>78</v>
+        <v>212</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>79</v>
+        <v>229</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>87</v>
+        <v>230</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>172</v>
+        <v>231</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW($A$3)</f>
         <v>24</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>78</v>
@@ -2449,25 +2496,25 @@
         <v>79</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>81</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW($A$3)</f>
         <v>25</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>78</v>
@@ -2476,25 +2523,25 @@
         <v>79</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>81</v>
       </c>
       <c r="H28" s="11" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW($A$3)</f>
         <v>26</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>156</v>
+        <v>85</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>157</v>
+        <v>86</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>78</v>
@@ -2503,52 +2550,52 @@
         <v>79</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>158</v>
+        <v>87</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>81</v>
       </c>
       <c r="H29" s="11" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="6">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW($A$3)</f>
         <v>27</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>225</v>
+        <v>88</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E30" s="9" t="s">
-        <v>159</v>
+      <c r="E30" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>160</v>
+        <v>90</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>81</v>
       </c>
       <c r="H30" s="11" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="6">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW($A$3)</f>
         <v>28</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>193</v>
+        <v>91</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>194</v>
+        <v>92</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>78</v>
@@ -2557,25 +2604,25 @@
         <v>79</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>226</v>
+        <v>93</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>81</v>
       </c>
       <c r="H31" s="11" t="s">
-        <v>227</v>
+        <v>174</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="6">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW($A$3)</f>
         <v>29</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>195</v>
+        <v>156</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>196</v>
+        <v>157</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>78</v>
@@ -2584,144 +2631,207 @@
         <v>79</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>197</v>
+        <v>158</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>81</v>
       </c>
       <c r="H32" s="11" t="s">
-        <v>198</v>
+        <v>175</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="6">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW($A$3)</f>
         <v>30</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>217</v>
+        <v>225</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>220</v>
+        <v>92</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E33" s="2" t="s">
-        <v>79</v>
+      <c r="E33" s="9" t="s">
+        <v>159</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>218</v>
+        <v>160</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>81</v>
       </c>
       <c r="H33" s="11" t="s">
-        <v>219</v>
+        <v>166</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="6">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW($A$3)</f>
         <v>31</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>161</v>
+        <v>193</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>163</v>
+        <v>194</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>164</v>
+        <v>78</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>162</v>
+        <v>226</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>81</v>
       </c>
       <c r="H34" s="11" t="s">
-        <v>165</v>
+        <v>227</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="6">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW($A$3)</f>
         <v>32</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>71</v>
+        <v>195</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>72</v>
+        <v>196</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>75</v>
+        <v>197</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="H35" s="11" t="s">
-        <v>167</v>
+        <v>198</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="6">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW($A$3)</f>
         <v>33</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>64</v>
+        <v>217</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>63</v>
+        <v>220</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>188</v>
+        <v>78</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>66</v>
+        <v>218</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="H36" s="11" t="s">
-        <v>65</v>
+        <v>219</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="6">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW($A$3)</f>
         <v>34</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H37" s="11" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="6">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW($A$3)</f>
         <v>35</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="H38" s="11" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="6">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW($A$3)</f>
         <v>36</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="6">
-        <f t="shared" si="0"/>
+        <f>ROW()-ROW($A$3)</f>
         <v>37</v>
       </c>
     </row>
@@ -2732,7 +2842,7 @@
     </sortState>
   </autoFilter>
   <hyperlinks>
-    <hyperlink ref="H22" r:id="rId1" xr:uid="{F87D5ED7-5837-4F4E-A63A-6E48CD176021}"/>
+    <hyperlink ref="H21" r:id="rId1" xr:uid="{F87D5ED7-5837-4F4E-A63A-6E48CD176021}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>